<commit_message>
2017 RevA boards complete
</commit_message>
<xml_diff>
--- a/PCB/BOM.xlsx
+++ b/PCB/BOM.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sensor" sheetId="1" r:id="rId1"/>
+    <sheet name="HAT" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="72">
   <si>
     <t>Part</t>
   </si>
@@ -184,6 +185,57 @@
   </si>
   <si>
     <t>R6</t>
+  </si>
+  <si>
+    <t>2x20 HAT Header</t>
+  </si>
+  <si>
+    <t>RTC</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/maxim-integrated/DS3231MZ/DS3231MZ-ND/2754396</t>
+  </si>
+  <si>
+    <t>DS3231MZ+</t>
+  </si>
+  <si>
+    <t>Backup Battery Holder</t>
+  </si>
+  <si>
+    <t>BAT-HLD-012-THM</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/linx-technologies-inc/BAT-HLD-012-THM/BAT-HLD-012-THM-ND/3044012</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/samtec-inc/SSQ-120-03-T-D/SAM1204-20-ND/1111840</t>
+  </si>
+  <si>
+    <t>SSQ-120-03-T-D</t>
+  </si>
+  <si>
+    <t>Decoupling Capacitor</t>
+  </si>
+  <si>
+    <t>CL21B104KBFNNNG</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/samsung-electro-mechanics/CL21B104KBFNNNG/1276-6468-1-ND/5958096</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>U4</t>
   </si>
 </sst>
 </file>
@@ -228,7 +280,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -236,8 +288,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -249,26 +332,82 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -292,16 +431,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G14" totalsRowShown="0">
-  <autoFilter ref="A1:G14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G15" totalsRowShown="0">
+  <autoFilter ref="A1:G15"/>
   <tableColumns count="7">
     <tableColumn id="7" name="Label"/>
     <tableColumn id="1" name="Description"/>
-    <tableColumn id="2" name="Part" dataDxfId="0"/>
+    <tableColumn id="2" name="Part" dataDxfId="2"/>
+    <tableColumn id="3" name="Quantity"/>
+    <tableColumn id="4" name="Unit Price"/>
+    <tableColumn id="5" name="Total Price" dataDxfId="0">
+      <calculatedColumnFormula>Table1[Unit Price]*Table1[Quantity]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="URL"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:G9" totalsRowShown="0">
+  <autoFilter ref="A1:G9"/>
+  <tableColumns count="7">
+    <tableColumn id="7" name="Label"/>
+    <tableColumn id="1" name="Description"/>
+    <tableColumn id="2" name="Part" dataDxfId="1"/>
     <tableColumn id="3" name="Quantity"/>
     <tableColumn id="4" name="Unit Price"/>
     <tableColumn id="5" name="Total Price">
-      <calculatedColumnFormula>Table1[Unit Price]*Table1[Quantity]</calculatedColumnFormula>
+      <calculatedColumnFormula>Table13[Unit Price]*Table13[Quantity]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" name="URL"/>
   </tableColumns>
@@ -634,7 +791,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -672,6 +829,9 @@
       </c>
     </row>
     <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
@@ -693,7 +853,9 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
@@ -715,7 +877,9 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
@@ -737,7 +901,9 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
@@ -968,13 +1134,37 @@
         <v>45</v>
       </c>
     </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="4">
+        <v>3</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="F15" s="4">
+        <f>Table1[Unit Price]*Table1[Quantity]</f>
+        <v>0.06</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
     <row r="20" spans="4:5">
       <c r="D20" t="s">
         <v>22</v>
       </c>
       <c r="E20">
         <f>SUM(Table1[Total Price])</f>
-        <v>9.7243999999999993</v>
+        <v>9.7843999999999998</v>
       </c>
     </row>
     <row r="21" spans="4:5">
@@ -991,7 +1181,275 @@
       </c>
       <c r="E22">
         <f>E20*E21</f>
-        <v>97.244</v>
+        <v>97.843999999999994</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="102" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2.62</v>
+      </c>
+      <c r="F2" s="2">
+        <f>Table13[Unit Price]*Table13[Quantity]</f>
+        <v>2.62</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.35120000000000001</v>
+      </c>
+      <c r="F3" s="2">
+        <f>Table13[Unit Price]*Table13[Quantity]</f>
+        <v>0.35120000000000001</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="2">
+        <v>4</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="F4" s="2">
+        <f>Table13[Unit Price]*Table13[Quantity]</f>
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="F5" s="2">
+        <f>Table13[Unit Price]*Table13[Quantity]</f>
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="F6" s="2">
+        <f>Table13[Unit Price]*Table13[Quantity]</f>
+        <v>4.5</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2">
+        <v>7.72</v>
+      </c>
+      <c r="F7" s="2">
+        <f>Table13[Unit Price]*Table13[Quantity]</f>
+        <v>7.72</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F8" s="2">
+        <f>Table13[Unit Price]*Table13[Quantity]</f>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="2">
+        <v>3</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="F9" s="2">
+        <f>Table13[Unit Price]*Table13[Quantity]</f>
+        <v>0.06</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12">
+        <f>SUM(Table13[Total Price])</f>
+        <v>15.653199999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="D14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14">
+        <f>E12*E13</f>
+        <v>15.653199999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed quantity on a couple components
</commit_message>
<xml_diff>
--- a/PCB/BOM.xlsx
+++ b/PCB/BOM.xlsx
@@ -320,8 +320,76 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -358,7 +426,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="95">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -372,6 +440,40 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -385,6 +487,40 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -1051,14 +1187,14 @@
         <v>39</v>
       </c>
       <c r="D11" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E11" s="2">
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="F11" s="2">
         <f>Table1[Unit Price]*Table1[Quantity]</f>
-        <v>4.3999999999999997E-2</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>40</v>
@@ -1075,14 +1211,14 @@
         <v>42</v>
       </c>
       <c r="D12" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12" s="2">
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="F12" s="2">
         <f>Table1[Unit Price]*Table1[Quantity]</f>
-        <v>1.7000000000000001E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>41</v>
@@ -1164,7 +1300,7 @@
       </c>
       <c r="E20">
         <f>SUM(Table1[Total Price])</f>
-        <v>9.7843999999999998</v>
+        <v>9.8453999999999997</v>
       </c>
     </row>
     <row r="21" spans="4:5">
@@ -1181,7 +1317,7 @@
       </c>
       <c r="E22">
         <f>E20*E21</f>
-        <v>97.843999999999994</v>
+        <v>98.453999999999994</v>
       </c>
     </row>
   </sheetData>
@@ -1203,7 +1339,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>